<commit_message>
Add metadata to the Project
</commit_message>
<xml_diff>
--- a/data/metadata.xlsx
+++ b/data/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9000"/>
+    <workbookView windowHeight="17640"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Charachteristics</t>
   </si>
@@ -35,22 +35,63 @@
     <t>Description</t>
   </si>
   <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Site and station codes</t>
+  </si>
+  <si>
+    <t>Site coding: River_Mesohabitat_SiteNumber (e.g., FR1 = Feng River, Rapid habitat, Site 1)
+Rivers: F=Feng, C=Chan, B=Ba, J=Jing, W=Wei
+Mesohabitats: R=Rapid, B=Benchland, P=Pool
+Sites: 1-9 per river (total 45 sites)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Zone</t>
+  </si>
+  <si>
+    <t>River Zone Codes: 
+Up = Upstream section
+Mid = Midstream section  
+Down = Downstream section</t>
+  </si>
+  <si>
     <t>Sediment chemistry</t>
   </si>
   <si>
     <t>S_TP = Sediment total Phosphorous, S_TN = Sediment Total Nitrogen, S_TOC = Sediment total organic carbon, S_moist = Soil moisture, S_pH= Soil pH</t>
   </si>
   <si>
+    <t>TP and TN mg/kg ; TOC and S_moist =%</t>
+  </si>
+  <si>
     <t>River and habitat charachteristics</t>
   </si>
   <si>
-    <t>length= mesohabitat length, width= mesohabitat width, r_width = river width</t>
+    <t>length or L = mesohabitat length, w or width= mesohabitat width, r_width = river width, river_chr = river charachteristics (PCA axis1)</t>
+  </si>
+  <si>
+    <t>meters (m)</t>
   </si>
   <si>
     <t>Soil and sediment charachteristics</t>
   </si>
   <si>
-    <t>v_course</t>
+    <t>1. GRANULE (GR): 2.0 - 4.0 mm
+2. SAND CLASSES:
+   • VCS: Very Coarse Sand (1.0 - 2.0 mm)
+   • CS: Coarse Sand (0.5 - 1.0 mm)
+   • MS: Medium Sand (0.25 - 0.5 mm)
+   • FS: Fine Sand (0.125 - 0.25 mm)
+   • VFS: Very Fine Sand (0.063 - 0.125 mm)
+3. FINE PARTICLES:
+   • SC: Silt and Clay (&lt; 0.063 mm)</t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
   <si>
     <t>Elevation</t>
@@ -62,13 +103,53 @@
     <t>Macroinvertebrate traits</t>
   </si>
   <si>
-    <t>FFG= Functional feeeding guilds, FC= Filter-collectors, GC=Gatherer-collectors, HSH=Sharaders, MF = Multi-functional feeding guilds, P= Predators, PR = Parasitic, PRC=Piercers, SC=Scrapers, BU=Burroers, CB = Climbers, CN= Clingers, SK= , SP = Sprawlers, MH= Multi-habit, CA=Carnivore, DE= Detritivores, DH= Detri-herbivores, HE= Herbivores, MT= Multi-trophic,</t>
+    <t>1. FUNCTIONAL FEEDING GUILDS (FFG)
+   • FC: Filterer-Collectors
+   • GC: Gatherer-Collectors  
+   • HSH: Shredders
+   • SC: Scrapers
+   • P: Predators
+   • PI: Piercers
+   • MF: Multi-functional
+   • PR: Parasites
+2. HABIT GROUPS (HG)
+   • BU: Burrowers
+   • CL: Climbers
+   • CN: Clingers
+   • SP: Sprawlers
+   • SW: Swimmers
+   • MH: Multi-habit
+3. TROPHIC GROUPS (TG)
+   • CA: Carnivores
+   • DE: Detritivores
+   • DH: Detri-Herbivores
+   • HE: Herbivores
+   • MT: Multi-trophic</t>
   </si>
   <si>
     <t>Diversity indices</t>
   </si>
   <si>
     <t>S=Species richness, N=Total number of individuals, d=Simpson’s diversity index, j=Pielou’s evenness, H=Shannon–Wiener diversity index</t>
+  </si>
+  <si>
+    <t>Macroinvertebrate species</t>
+  </si>
+  <si>
+    <t>Total count per species (Density) and abundance</t>
+  </si>
+  <si>
+    <t>Individual per square meter (Individuals/m²)</t>
+  </si>
+  <si>
+    <t>DATA STRUCTURE:
+Rows: Each row = one sampling site 
+Columns: 
+Col1: Site ID
+Col2: HabitatType (R=Rapid, B=Benchland, P=Pool)
+Col3+: Environmental variables (units) OR Species data (abundance/measurements)
+RIVER CODES: F=Feng, C=Chan, B=Ba, J=Jing, W=Wei
+ZONE CODES: Up=Upstream, Mid=Midstream, Down=Downstream</t>
   </si>
 </sst>
 </file>
@@ -81,7 +162,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +186,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -443,12 +532,160 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="23">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -569,151 +806,193 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1248,75 +1527,179 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="37.5555555555556" customWidth="1"/>
     <col min="2" max="2" width="53.1111111111111" customWidth="1"/>
+    <col min="3" max="3" width="43.4444444444444" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="1" ht="15.6" spans="1:3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" ht="46.8" spans="1:2">
-      <c r="A2" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+    </row>
+    <row r="2" ht="78" spans="1:3">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" ht="31.2" spans="1:2">
-      <c r="A3" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="15.6" spans="1:2">
-      <c r="A4" s="3" t="s">
+    <row r="3" ht="62.4" spans="1:3">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" ht="31.2" spans="1:2">
-      <c r="A5" s="3" t="s">
+      <c r="C3" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" ht="46.8" spans="1:3">
+      <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" ht="109.2" spans="1:2">
-      <c r="A6" s="3" t="s">
+      <c r="C4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="4" t="s">
+    </row>
+    <row r="5" ht="46.8" spans="1:3">
+      <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" ht="46.8" spans="1:2">
-      <c r="A7" s="3" t="s">
+      <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C5" s="9" t="s">
         <v>13</v>
       </c>
     </row>
+    <row r="6" ht="140.4" spans="1:3">
+      <c r="A6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" ht="31.2" spans="1:3">
+      <c r="A7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" ht="374.4" spans="1:3">
+      <c r="A8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="9"/>
+    </row>
+    <row r="9" ht="46.8" spans="1:3">
+      <c r="A9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="9"/>
+    </row>
+    <row r="10" ht="16.35" spans="1:3">
+      <c r="A10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" ht="15.6" spans="1:2">
+      <c r="A14" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="14"/>
+    </row>
+    <row r="15" ht="15.6" spans="1:2">
+      <c r="A15" s="15"/>
+      <c r="B15" s="16"/>
+    </row>
+    <row r="16" ht="15.6" spans="1:2">
+      <c r="A16" s="15"/>
+      <c r="B16" s="16"/>
+    </row>
+    <row r="17" ht="15.6" spans="1:2">
+      <c r="A17" s="15"/>
+      <c r="B17" s="16"/>
+    </row>
+    <row r="18" ht="15.6" spans="1:2">
+      <c r="A18" s="15"/>
+      <c r="B18" s="16"/>
+    </row>
+    <row r="19" ht="15.6" spans="1:2">
+      <c r="A19" s="15"/>
+      <c r="B19" s="16"/>
+    </row>
+    <row r="20" ht="15.6" spans="1:2">
+      <c r="A20" s="15"/>
+      <c r="B20" s="16"/>
+    </row>
+    <row r="21" ht="15.6" spans="1:2">
+      <c r="A21" s="15"/>
+      <c r="B21" s="16"/>
+    </row>
+    <row r="22" ht="15.6" spans="1:2">
+      <c r="A22" s="15"/>
+      <c r="B22" s="16"/>
+    </row>
+    <row r="23" ht="15.6" spans="1:2">
+      <c r="A23" s="15"/>
+      <c r="B23" s="16"/>
+    </row>
+    <row r="24" ht="15.6" spans="1:2">
+      <c r="A24" s="15"/>
+      <c r="B24" s="16"/>
+    </row>
+    <row r="25" ht="15.6" spans="1:2">
+      <c r="A25" s="17"/>
+      <c r="B25" s="18"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A14:B25"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>